<commit_message>
update raw GLG data
</commit_message>
<xml_diff>
--- a/data/raw/FormBased_FieldMedicalPFAStudy.xlsx
+++ b/data/raw/FormBased_FieldMedicalPFAStudy.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathansalas/R_Projects/VCAS1_prelim_efficiency/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5945988-8960-E147-A182-658C3EF623C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D60DBD6-CAC8-0446-9560-2081840D9AC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="F14-Index Procedure for VT" sheetId="2" r:id="rId1"/>
+    <sheet name="F14-Index Procedure for VT" sheetId="4" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3239" uniqueCount="603">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3636" uniqueCount="653">
   <si>
     <t>Date and time that the form answers were created (first save) in Greenlight Guru Clinical</t>
   </si>
@@ -1829,6 +1829,156 @@
   </si>
   <si>
     <t>CL13792-10</t>
+  </si>
+  <si>
+    <t>6853974a18d04920b3aa51a6</t>
+  </si>
+  <si>
+    <t>1-026</t>
+  </si>
+  <si>
+    <t>05:25</t>
+  </si>
+  <si>
+    <t>001-026_Procedure_ECG.pdf</t>
+  </si>
+  <si>
+    <t>21:49</t>
+  </si>
+  <si>
+    <t>22:17</t>
+  </si>
+  <si>
+    <t>23:05</t>
+  </si>
+  <si>
+    <t>23:08</t>
+  </si>
+  <si>
+    <t>23:57</t>
+  </si>
+  <si>
+    <t>120 mg</t>
+  </si>
+  <si>
+    <t>23:58</t>
+  </si>
+  <si>
+    <t>mg/dL</t>
+  </si>
+  <si>
+    <t>CL13878-3</t>
+  </si>
+  <si>
+    <t>10911</t>
+  </si>
+  <si>
+    <t>24FFFGEN003 1.0.3</t>
+  </si>
+  <si>
+    <t>685be08329bd4c5dd0cf9b11</t>
+  </si>
+  <si>
+    <t>3-005</t>
+  </si>
+  <si>
+    <t>Incomplete</t>
+  </si>
+  <si>
+    <t>08:23</t>
+  </si>
+  <si>
+    <t>03-005_ECG_before ablation.pdf</t>
+  </si>
+  <si>
+    <t>08:30</t>
+  </si>
+  <si>
+    <t>08:51</t>
+  </si>
+  <si>
+    <t>08:44</t>
+  </si>
+  <si>
+    <t>09:27</t>
+  </si>
+  <si>
+    <t>09:58</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>i.v</t>
+  </si>
+  <si>
+    <t>10:02</t>
+  </si>
+  <si>
+    <t>A11218</t>
+  </si>
+  <si>
+    <t>1.2.2</t>
+  </si>
+  <si>
+    <t>6863c9c3d2b0b40d10dcaf61</t>
+  </si>
+  <si>
+    <t>3-006</t>
+  </si>
+  <si>
+    <t>10:57</t>
+  </si>
+  <si>
+    <t>3-006_ECG_V1ABL.pdf</t>
+  </si>
+  <si>
+    <t>11:17</t>
+  </si>
+  <si>
+    <t>11:52</t>
+  </si>
+  <si>
+    <t>12:15</t>
+  </si>
+  <si>
+    <t>12:16</t>
+  </si>
+  <si>
+    <t>12:54</t>
+  </si>
+  <si>
+    <t>12:56</t>
+  </si>
+  <si>
+    <t>6863cda3d2b0b40d10e0084d</t>
+  </si>
+  <si>
+    <t>3-008</t>
+  </si>
+  <si>
+    <t>3-008_V1ABL.pdf</t>
+  </si>
+  <si>
+    <t>11:21</t>
+  </si>
+  <si>
+    <t>11:56</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>12:33</t>
+  </si>
+  <si>
+    <t>CL13878-17</t>
+  </si>
+  <si>
+    <t>CL13792 -21; CL13792-16</t>
+  </si>
+  <si>
+    <t>CL13792-15</t>
   </si>
 </sst>
 </file>
@@ -2172,8 +2322,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:DH32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11D1BF5A-D059-3844-BFF6-BE5FC0167D64}">
+  <dimension ref="A1:DH36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -7544,7 +7694,7 @@
         <v>45510.279826388898</v>
       </c>
       <c r="G17" s="1">
-        <v>45614.483009259297</v>
+        <v>45859.0629050926</v>
       </c>
       <c r="H17" t="s">
         <v>235</v>
@@ -7652,7 +7802,7 @@
         <v>244</v>
       </c>
       <c r="AQ17">
-        <v>10</v>
+        <v>105</v>
       </c>
       <c r="AR17">
         <v>21</v>
@@ -8205,7 +8355,7 @@
         <v>442</v>
       </c>
       <c r="B19" t="s">
-        <v>379</v>
+        <v>233</v>
       </c>
       <c r="C19" t="s">
         <v>443</v>
@@ -8213,8 +8363,8 @@
       <c r="D19" s="1">
         <v>45590.086377314801</v>
       </c>
-      <c r="E19" t="s">
-        <v>261</v>
+      <c r="E19" s="1">
+        <v>45789.165162037003</v>
       </c>
       <c r="F19" s="1">
         <v>45590.136631944399</v>
@@ -9895,7 +10045,7 @@
         <v>508</v>
       </c>
       <c r="B24" t="s">
-        <v>379</v>
+        <v>233</v>
       </c>
       <c r="C24" t="s">
         <v>509</v>
@@ -9903,8 +10053,8 @@
       <c r="D24" s="1">
         <v>45616.428888888899</v>
       </c>
-      <c r="E24" t="s">
-        <v>261</v>
+      <c r="E24" s="1">
+        <v>45798.366620370398</v>
       </c>
       <c r="F24" s="1">
         <v>45627.543425925898</v>
@@ -10233,7 +10383,7 @@
         <v>519</v>
       </c>
       <c r="B25" t="s">
-        <v>379</v>
+        <v>233</v>
       </c>
       <c r="C25" t="s">
         <v>520</v>
@@ -10241,8 +10391,8 @@
       <c r="D25" s="1">
         <v>45621.445196759298</v>
       </c>
-      <c r="E25" t="s">
-        <v>261</v>
+      <c r="E25" s="1">
+        <v>45793.0629976852</v>
       </c>
       <c r="F25" s="1">
         <v>45622.155624999999</v>
@@ -10571,7 +10721,7 @@
         <v>531</v>
       </c>
       <c r="B26" t="s">
-        <v>379</v>
+        <v>233</v>
       </c>
       <c r="C26" t="s">
         <v>532</v>
@@ -10579,8 +10729,8 @@
       <c r="D26" s="1">
         <v>45621.4453125</v>
       </c>
-      <c r="E26" t="s">
-        <v>261</v>
+      <c r="E26" s="1">
+        <v>45789.071562500001</v>
       </c>
       <c r="F26" s="1">
         <v>45622.226689814801</v>
@@ -10909,7 +11059,7 @@
         <v>541</v>
       </c>
       <c r="B27" t="s">
-        <v>379</v>
+        <v>233</v>
       </c>
       <c r="C27" t="s">
         <v>542</v>
@@ -10917,8 +11067,8 @@
       <c r="D27" s="1">
         <v>45666.052847222199</v>
       </c>
-      <c r="E27" t="s">
-        <v>261</v>
+      <c r="E27" s="1">
+        <v>45793.065671296303</v>
       </c>
       <c r="F27" s="1">
         <v>45666.335763888899</v>
@@ -11585,7 +11735,7 @@
         <v>560</v>
       </c>
       <c r="B29" t="s">
-        <v>379</v>
+        <v>233</v>
       </c>
       <c r="C29" t="s">
         <v>561</v>
@@ -11593,8 +11743,8 @@
       <c r="D29" s="1">
         <v>45666.052986111099</v>
       </c>
-      <c r="E29" t="s">
-        <v>261</v>
+      <c r="E29" s="1">
+        <v>45845.222048611096</v>
       </c>
       <c r="F29" s="1">
         <v>45667.0333680556</v>
@@ -11923,7 +12073,7 @@
         <v>573</v>
       </c>
       <c r="B30" t="s">
-        <v>379</v>
+        <v>233</v>
       </c>
       <c r="C30" t="s">
         <v>574</v>
@@ -11931,8 +12081,8 @@
       <c r="D30" s="1">
         <v>45666.053055555603</v>
       </c>
-      <c r="E30" t="s">
-        <v>261</v>
+      <c r="E30" s="1">
+        <v>45838.277893518498</v>
       </c>
       <c r="F30" s="1">
         <v>45667.081122685202</v>
@@ -12929,6 +13079,1358 @@
         <v>282</v>
       </c>
       <c r="DH32" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="33" spans="1:112" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>603</v>
+      </c>
+      <c r="B33" t="s">
+        <v>379</v>
+      </c>
+      <c r="C33" t="s">
+        <v>604</v>
+      </c>
+      <c r="D33" s="1">
+        <v>45827.035671296297</v>
+      </c>
+      <c r="E33" t="s">
+        <v>261</v>
+      </c>
+      <c r="F33" s="1">
+        <v>45835.212025462999</v>
+      </c>
+      <c r="G33" s="1">
+        <v>45835.212025462999</v>
+      </c>
+      <c r="H33" t="s">
+        <v>235</v>
+      </c>
+      <c r="I33" s="1">
+        <v>45827.035338449103</v>
+      </c>
+      <c r="J33" t="s">
+        <v>236</v>
+      </c>
+      <c r="K33" t="s">
+        <v>237</v>
+      </c>
+      <c r="L33" t="s">
+        <v>238</v>
+      </c>
+      <c r="M33" s="2">
+        <v>45828</v>
+      </c>
+      <c r="N33" t="s">
+        <v>239</v>
+      </c>
+      <c r="O33" t="s">
+        <v>240</v>
+      </c>
+      <c r="P33" t="s">
+        <v>605</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>606</v>
+      </c>
+      <c r="R33" t="s">
+        <v>607</v>
+      </c>
+      <c r="S33" t="s">
+        <v>239</v>
+      </c>
+      <c r="T33" t="s">
+        <v>244</v>
+      </c>
+      <c r="U33">
+        <v>304</v>
+      </c>
+      <c r="V33" t="s">
+        <v>245</v>
+      </c>
+      <c r="W33" t="s">
+        <v>608</v>
+      </c>
+      <c r="X33" t="s">
+        <v>247</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>248</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>240</v>
+      </c>
+      <c r="AA33" t="s">
+        <v>249</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>274</v>
+      </c>
+      <c r="AC33" t="s">
+        <v>239</v>
+      </c>
+      <c r="AD33" t="s">
+        <v>609</v>
+      </c>
+      <c r="AE33" t="s">
+        <v>610</v>
+      </c>
+      <c r="AF33" t="s">
+        <v>247</v>
+      </c>
+      <c r="AG33" t="s">
+        <v>248</v>
+      </c>
+      <c r="AH33" t="s">
+        <v>247</v>
+      </c>
+      <c r="AI33" t="s">
+        <v>253</v>
+      </c>
+      <c r="AJ33" t="s">
+        <v>247</v>
+      </c>
+      <c r="AK33" t="s">
+        <v>244</v>
+      </c>
+      <c r="AL33" t="s">
+        <v>449</v>
+      </c>
+      <c r="AM33">
+        <v>15</v>
+      </c>
+      <c r="AN33" t="s">
+        <v>611</v>
+      </c>
+      <c r="AO33" t="s">
+        <v>240</v>
+      </c>
+      <c r="AP33" t="s">
+        <v>244</v>
+      </c>
+      <c r="AQ33">
+        <v>125</v>
+      </c>
+      <c r="AR33">
+        <v>25</v>
+      </c>
+      <c r="AS33" t="s">
+        <v>239</v>
+      </c>
+      <c r="AT33" t="s">
+        <v>257</v>
+      </c>
+      <c r="AU33" t="s">
+        <v>247</v>
+      </c>
+      <c r="AV33" t="s">
+        <v>247</v>
+      </c>
+      <c r="AW33" t="s">
+        <v>247</v>
+      </c>
+      <c r="AX33" t="s">
+        <v>244</v>
+      </c>
+      <c r="AY33" t="s">
+        <v>258</v>
+      </c>
+      <c r="AZ33" t="s">
+        <v>612</v>
+      </c>
+      <c r="BA33" t="s">
+        <v>260</v>
+      </c>
+      <c r="BB33" t="s">
+        <v>261</v>
+      </c>
+      <c r="BC33" t="s">
+        <v>261</v>
+      </c>
+      <c r="BD33" t="s">
+        <v>261</v>
+      </c>
+      <c r="BE33" t="s">
+        <v>261</v>
+      </c>
+      <c r="BF33" t="s">
+        <v>261</v>
+      </c>
+      <c r="BG33" t="s">
+        <v>261</v>
+      </c>
+      <c r="BH33" t="s">
+        <v>261</v>
+      </c>
+      <c r="BI33" t="s">
+        <v>261</v>
+      </c>
+      <c r="BJ33" t="s">
+        <v>261</v>
+      </c>
+      <c r="BK33" t="s">
+        <v>261</v>
+      </c>
+      <c r="BL33" t="s">
+        <v>261</v>
+      </c>
+      <c r="BM33" t="s">
+        <v>261</v>
+      </c>
+      <c r="BN33" t="s">
+        <v>261</v>
+      </c>
+      <c r="BO33" t="s">
+        <v>261</v>
+      </c>
+      <c r="BP33" t="s">
+        <v>261</v>
+      </c>
+      <c r="BQ33" t="s">
+        <v>261</v>
+      </c>
+      <c r="BR33" t="s">
+        <v>261</v>
+      </c>
+      <c r="BS33" t="s">
+        <v>261</v>
+      </c>
+      <c r="BT33" t="s">
+        <v>261</v>
+      </c>
+      <c r="BU33" t="s">
+        <v>261</v>
+      </c>
+      <c r="BV33" t="s">
+        <v>261</v>
+      </c>
+      <c r="BW33" t="s">
+        <v>261</v>
+      </c>
+      <c r="BX33" t="s">
+        <v>261</v>
+      </c>
+      <c r="BY33" t="s">
+        <v>261</v>
+      </c>
+      <c r="BZ33" t="s">
+        <v>261</v>
+      </c>
+      <c r="CA33" t="s">
+        <v>261</v>
+      </c>
+      <c r="CB33" t="s">
+        <v>261</v>
+      </c>
+      <c r="CC33" t="s">
+        <v>261</v>
+      </c>
+      <c r="CD33" t="s">
+        <v>261</v>
+      </c>
+      <c r="CE33" t="s">
+        <v>261</v>
+      </c>
+      <c r="CF33" t="s">
+        <v>261</v>
+      </c>
+      <c r="CG33" t="s">
+        <v>261</v>
+      </c>
+      <c r="CH33" t="s">
+        <v>261</v>
+      </c>
+      <c r="CI33" t="s">
+        <v>261</v>
+      </c>
+      <c r="CJ33" t="s">
+        <v>261</v>
+      </c>
+      <c r="CK33" t="s">
+        <v>261</v>
+      </c>
+      <c r="CL33" t="s">
+        <v>261</v>
+      </c>
+      <c r="CM33" t="s">
+        <v>261</v>
+      </c>
+      <c r="CN33" t="s">
+        <v>261</v>
+      </c>
+      <c r="CO33" t="s">
+        <v>261</v>
+      </c>
+      <c r="CP33" t="s">
+        <v>261</v>
+      </c>
+      <c r="CQ33" t="s">
+        <v>261</v>
+      </c>
+      <c r="CR33">
+        <v>3</v>
+      </c>
+      <c r="CS33" t="s">
+        <v>613</v>
+      </c>
+      <c r="CT33">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="CU33" t="s">
+        <v>614</v>
+      </c>
+      <c r="CV33" t="s">
+        <v>239</v>
+      </c>
+      <c r="CW33" t="s">
+        <v>244</v>
+      </c>
+      <c r="CX33" t="s">
+        <v>244</v>
+      </c>
+      <c r="CY33" t="s">
+        <v>244</v>
+      </c>
+      <c r="CZ33" t="s">
+        <v>244</v>
+      </c>
+      <c r="DA33" t="s">
+        <v>239</v>
+      </c>
+      <c r="DB33" t="s">
+        <v>244</v>
+      </c>
+      <c r="DC33" t="s">
+        <v>615</v>
+      </c>
+      <c r="DD33" t="s">
+        <v>282</v>
+      </c>
+      <c r="DE33" t="s">
+        <v>616</v>
+      </c>
+      <c r="DF33" t="s">
+        <v>617</v>
+      </c>
+      <c r="DG33" t="s">
+        <v>282</v>
+      </c>
+      <c r="DH33" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="34" spans="1:112" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>618</v>
+      </c>
+      <c r="B34" t="s">
+        <v>379</v>
+      </c>
+      <c r="C34" t="s">
+        <v>619</v>
+      </c>
+      <c r="D34" s="1">
+        <v>45833.320775462998</v>
+      </c>
+      <c r="E34" t="s">
+        <v>261</v>
+      </c>
+      <c r="F34" s="1">
+        <v>45838.377199074101</v>
+      </c>
+      <c r="G34" s="1">
+        <v>45856.285856481503</v>
+      </c>
+      <c r="H34" t="s">
+        <v>235</v>
+      </c>
+      <c r="I34" s="1">
+        <v>45833.320437256902</v>
+      </c>
+      <c r="J34" t="s">
+        <v>620</v>
+      </c>
+      <c r="K34" t="s">
+        <v>237</v>
+      </c>
+      <c r="L34" t="s">
+        <v>238</v>
+      </c>
+      <c r="M34" s="2">
+        <v>45831</v>
+      </c>
+      <c r="N34" t="s">
+        <v>239</v>
+      </c>
+      <c r="O34" t="s">
+        <v>240</v>
+      </c>
+      <c r="P34" t="s">
+        <v>621</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>622</v>
+      </c>
+      <c r="R34" t="s">
+        <v>623</v>
+      </c>
+      <c r="S34" t="s">
+        <v>239</v>
+      </c>
+      <c r="T34" t="s">
+        <v>244</v>
+      </c>
+      <c r="U34">
+        <v>331</v>
+      </c>
+      <c r="V34" t="s">
+        <v>245</v>
+      </c>
+      <c r="W34" t="s">
+        <v>624</v>
+      </c>
+      <c r="X34" t="s">
+        <v>247</v>
+      </c>
+      <c r="Y34" t="s">
+        <v>248</v>
+      </c>
+      <c r="Z34" t="s">
+        <v>240</v>
+      </c>
+      <c r="AA34" t="s">
+        <v>249</v>
+      </c>
+      <c r="AB34" t="s">
+        <v>625</v>
+      </c>
+      <c r="AC34" t="s">
+        <v>261</v>
+      </c>
+      <c r="AD34" t="s">
+        <v>626</v>
+      </c>
+      <c r="AE34" t="s">
+        <v>250</v>
+      </c>
+      <c r="AF34" t="s">
+        <v>247</v>
+      </c>
+      <c r="AG34" t="s">
+        <v>248</v>
+      </c>
+      <c r="AH34" t="s">
+        <v>247</v>
+      </c>
+      <c r="AI34" t="s">
+        <v>253</v>
+      </c>
+      <c r="AJ34" t="s">
+        <v>247</v>
+      </c>
+      <c r="AK34" t="s">
+        <v>244</v>
+      </c>
+      <c r="AL34" t="s">
+        <v>449</v>
+      </c>
+      <c r="AM34">
+        <v>15</v>
+      </c>
+      <c r="AN34" t="s">
+        <v>627</v>
+      </c>
+      <c r="AO34" t="s">
+        <v>240</v>
+      </c>
+      <c r="AP34" t="s">
+        <v>244</v>
+      </c>
+      <c r="AQ34">
+        <v>45</v>
+      </c>
+      <c r="AR34">
+        <v>9</v>
+      </c>
+      <c r="AS34" t="s">
+        <v>239</v>
+      </c>
+      <c r="AT34" t="s">
+        <v>257</v>
+      </c>
+      <c r="AU34" t="s">
+        <v>247</v>
+      </c>
+      <c r="AV34" t="s">
+        <v>247</v>
+      </c>
+      <c r="AW34" t="s">
+        <v>247</v>
+      </c>
+      <c r="AX34" t="s">
+        <v>244</v>
+      </c>
+      <c r="AY34" t="s">
+        <v>258</v>
+      </c>
+      <c r="AZ34" t="s">
+        <v>628</v>
+      </c>
+      <c r="BA34" t="s">
+        <v>629</v>
+      </c>
+      <c r="BB34" t="s">
+        <v>261</v>
+      </c>
+      <c r="BC34" t="s">
+        <v>261</v>
+      </c>
+      <c r="BD34" t="s">
+        <v>261</v>
+      </c>
+      <c r="BE34" t="s">
+        <v>261</v>
+      </c>
+      <c r="BF34" t="s">
+        <v>261</v>
+      </c>
+      <c r="BG34" t="s">
+        <v>261</v>
+      </c>
+      <c r="BH34" t="s">
+        <v>261</v>
+      </c>
+      <c r="BI34" t="s">
+        <v>261</v>
+      </c>
+      <c r="BJ34" t="s">
+        <v>261</v>
+      </c>
+      <c r="BK34" t="s">
+        <v>261</v>
+      </c>
+      <c r="BL34" t="s">
+        <v>261</v>
+      </c>
+      <c r="BM34" t="s">
+        <v>261</v>
+      </c>
+      <c r="BN34" t="s">
+        <v>261</v>
+      </c>
+      <c r="BO34" t="s">
+        <v>261</v>
+      </c>
+      <c r="BP34" t="s">
+        <v>261</v>
+      </c>
+      <c r="BQ34" t="s">
+        <v>261</v>
+      </c>
+      <c r="BR34" t="s">
+        <v>261</v>
+      </c>
+      <c r="BS34" t="s">
+        <v>261</v>
+      </c>
+      <c r="BT34" t="s">
+        <v>261</v>
+      </c>
+      <c r="BU34" t="s">
+        <v>261</v>
+      </c>
+      <c r="BV34" t="s">
+        <v>261</v>
+      </c>
+      <c r="BW34" t="s">
+        <v>261</v>
+      </c>
+      <c r="BX34" t="s">
+        <v>261</v>
+      </c>
+      <c r="BY34" t="s">
+        <v>261</v>
+      </c>
+      <c r="BZ34" t="s">
+        <v>261</v>
+      </c>
+      <c r="CA34" t="s">
+        <v>261</v>
+      </c>
+      <c r="CB34" t="s">
+        <v>261</v>
+      </c>
+      <c r="CC34" t="s">
+        <v>261</v>
+      </c>
+      <c r="CD34" t="s">
+        <v>261</v>
+      </c>
+      <c r="CE34" t="s">
+        <v>261</v>
+      </c>
+      <c r="CF34" t="s">
+        <v>261</v>
+      </c>
+      <c r="CG34" t="s">
+        <v>261</v>
+      </c>
+      <c r="CH34" t="s">
+        <v>261</v>
+      </c>
+      <c r="CI34" t="s">
+        <v>261</v>
+      </c>
+      <c r="CJ34" t="s">
+        <v>261</v>
+      </c>
+      <c r="CK34" t="s">
+        <v>261</v>
+      </c>
+      <c r="CL34" t="s">
+        <v>261</v>
+      </c>
+      <c r="CM34" t="s">
+        <v>261</v>
+      </c>
+      <c r="CN34" t="s">
+        <v>261</v>
+      </c>
+      <c r="CO34" t="s">
+        <v>261</v>
+      </c>
+      <c r="CP34" t="s">
+        <v>261</v>
+      </c>
+      <c r="CQ34" t="s">
+        <v>261</v>
+      </c>
+      <c r="CR34">
+        <v>6.5</v>
+      </c>
+      <c r="CS34" t="s">
+        <v>630</v>
+      </c>
+      <c r="CT34">
+        <v>0.75</v>
+      </c>
+      <c r="CU34" t="s">
+        <v>280</v>
+      </c>
+      <c r="CV34" t="s">
+        <v>239</v>
+      </c>
+      <c r="CW34" t="s">
+        <v>244</v>
+      </c>
+      <c r="CX34" t="s">
+        <v>244</v>
+      </c>
+      <c r="CY34" t="s">
+        <v>244</v>
+      </c>
+      <c r="CZ34" t="s">
+        <v>244</v>
+      </c>
+      <c r="DA34" t="s">
+        <v>239</v>
+      </c>
+      <c r="DB34" t="s">
+        <v>244</v>
+      </c>
+      <c r="DC34" t="s">
+        <v>650</v>
+      </c>
+      <c r="DD34" t="s">
+        <v>282</v>
+      </c>
+      <c r="DE34" t="s">
+        <v>631</v>
+      </c>
+      <c r="DF34" t="s">
+        <v>632</v>
+      </c>
+      <c r="DG34" t="s">
+        <v>282</v>
+      </c>
+      <c r="DH34" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="35" spans="1:112" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>633</v>
+      </c>
+      <c r="B35" t="s">
+        <v>379</v>
+      </c>
+      <c r="C35" t="s">
+        <v>634</v>
+      </c>
+      <c r="D35" s="1">
+        <v>45839.321516203701</v>
+      </c>
+      <c r="E35" t="s">
+        <v>261</v>
+      </c>
+      <c r="F35" s="1">
+        <v>45840.253634259301</v>
+      </c>
+      <c r="G35" s="1">
+        <v>45856.280636574098</v>
+      </c>
+      <c r="H35" t="s">
+        <v>235</v>
+      </c>
+      <c r="I35" s="1">
+        <v>45839.321179884297</v>
+      </c>
+      <c r="J35" t="s">
+        <v>620</v>
+      </c>
+      <c r="K35" t="s">
+        <v>237</v>
+      </c>
+      <c r="L35" t="s">
+        <v>238</v>
+      </c>
+      <c r="M35" s="2">
+        <v>45831</v>
+      </c>
+      <c r="N35" t="s">
+        <v>239</v>
+      </c>
+      <c r="O35" t="s">
+        <v>240</v>
+      </c>
+      <c r="P35" t="s">
+        <v>635</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>636</v>
+      </c>
+      <c r="R35" t="s">
+        <v>637</v>
+      </c>
+      <c r="S35" t="s">
+        <v>239</v>
+      </c>
+      <c r="T35" t="s">
+        <v>244</v>
+      </c>
+      <c r="U35">
+        <v>314</v>
+      </c>
+      <c r="V35" t="s">
+        <v>245</v>
+      </c>
+      <c r="W35" t="s">
+        <v>638</v>
+      </c>
+      <c r="X35" t="s">
+        <v>247</v>
+      </c>
+      <c r="Y35" t="s">
+        <v>248</v>
+      </c>
+      <c r="Z35" t="s">
+        <v>240</v>
+      </c>
+      <c r="AA35" t="s">
+        <v>249</v>
+      </c>
+      <c r="AB35" t="s">
+        <v>537</v>
+      </c>
+      <c r="AC35" t="s">
+        <v>261</v>
+      </c>
+      <c r="AD35" t="s">
+        <v>639</v>
+      </c>
+      <c r="AE35" t="s">
+        <v>640</v>
+      </c>
+      <c r="AF35" t="s">
+        <v>247</v>
+      </c>
+      <c r="AG35" t="s">
+        <v>248</v>
+      </c>
+      <c r="AH35" t="s">
+        <v>247</v>
+      </c>
+      <c r="AI35" t="s">
+        <v>253</v>
+      </c>
+      <c r="AJ35" t="s">
+        <v>247</v>
+      </c>
+      <c r="AK35" t="s">
+        <v>244</v>
+      </c>
+      <c r="AL35" t="s">
+        <v>449</v>
+      </c>
+      <c r="AM35">
+        <v>15</v>
+      </c>
+      <c r="AN35" t="s">
+        <v>641</v>
+      </c>
+      <c r="AO35" t="s">
+        <v>240</v>
+      </c>
+      <c r="AP35" t="s">
+        <v>244</v>
+      </c>
+      <c r="AQ35">
+        <v>71</v>
+      </c>
+      <c r="AR35">
+        <v>14</v>
+      </c>
+      <c r="AS35" t="s">
+        <v>239</v>
+      </c>
+      <c r="AT35" t="s">
+        <v>257</v>
+      </c>
+      <c r="AU35" t="s">
+        <v>247</v>
+      </c>
+      <c r="AV35" t="s">
+        <v>247</v>
+      </c>
+      <c r="AW35" t="s">
+        <v>247</v>
+      </c>
+      <c r="AX35" t="s">
+        <v>244</v>
+      </c>
+      <c r="AY35" t="s">
+        <v>258</v>
+      </c>
+      <c r="AZ35" t="s">
+        <v>628</v>
+      </c>
+      <c r="BA35" t="s">
+        <v>629</v>
+      </c>
+      <c r="BB35" t="s">
+        <v>261</v>
+      </c>
+      <c r="BC35" t="s">
+        <v>261</v>
+      </c>
+      <c r="BD35" t="s">
+        <v>261</v>
+      </c>
+      <c r="BE35" t="s">
+        <v>261</v>
+      </c>
+      <c r="BF35" t="s">
+        <v>261</v>
+      </c>
+      <c r="BG35" t="s">
+        <v>261</v>
+      </c>
+      <c r="BH35" t="s">
+        <v>261</v>
+      </c>
+      <c r="BI35" t="s">
+        <v>261</v>
+      </c>
+      <c r="BJ35" t="s">
+        <v>261</v>
+      </c>
+      <c r="BK35" t="s">
+        <v>261</v>
+      </c>
+      <c r="BL35" t="s">
+        <v>261</v>
+      </c>
+      <c r="BM35" t="s">
+        <v>261</v>
+      </c>
+      <c r="BN35" t="s">
+        <v>261</v>
+      </c>
+      <c r="BO35" t="s">
+        <v>261</v>
+      </c>
+      <c r="BP35" t="s">
+        <v>261</v>
+      </c>
+      <c r="BQ35" t="s">
+        <v>261</v>
+      </c>
+      <c r="BR35" t="s">
+        <v>261</v>
+      </c>
+      <c r="BS35" t="s">
+        <v>261</v>
+      </c>
+      <c r="BT35" t="s">
+        <v>261</v>
+      </c>
+      <c r="BU35" t="s">
+        <v>261</v>
+      </c>
+      <c r="BV35" t="s">
+        <v>261</v>
+      </c>
+      <c r="BW35" t="s">
+        <v>261</v>
+      </c>
+      <c r="BX35" t="s">
+        <v>261</v>
+      </c>
+      <c r="BY35" t="s">
+        <v>261</v>
+      </c>
+      <c r="BZ35" t="s">
+        <v>261</v>
+      </c>
+      <c r="CA35" t="s">
+        <v>261</v>
+      </c>
+      <c r="CB35" t="s">
+        <v>261</v>
+      </c>
+      <c r="CC35" t="s">
+        <v>261</v>
+      </c>
+      <c r="CD35" t="s">
+        <v>261</v>
+      </c>
+      <c r="CE35" t="s">
+        <v>261</v>
+      </c>
+      <c r="CF35" t="s">
+        <v>261</v>
+      </c>
+      <c r="CG35" t="s">
+        <v>261</v>
+      </c>
+      <c r="CH35" t="s">
+        <v>261</v>
+      </c>
+      <c r="CI35" t="s">
+        <v>261</v>
+      </c>
+      <c r="CJ35" t="s">
+        <v>261</v>
+      </c>
+      <c r="CK35" t="s">
+        <v>261</v>
+      </c>
+      <c r="CL35" t="s">
+        <v>261</v>
+      </c>
+      <c r="CM35" t="s">
+        <v>261</v>
+      </c>
+      <c r="CN35" t="s">
+        <v>261</v>
+      </c>
+      <c r="CO35" t="s">
+        <v>261</v>
+      </c>
+      <c r="CP35" t="s">
+        <v>261</v>
+      </c>
+      <c r="CQ35" t="s">
+        <v>261</v>
+      </c>
+      <c r="CR35">
+        <v>3.9</v>
+      </c>
+      <c r="CS35" t="s">
+        <v>642</v>
+      </c>
+      <c r="CT35">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="CU35" t="s">
+        <v>280</v>
+      </c>
+      <c r="CV35" t="s">
+        <v>239</v>
+      </c>
+      <c r="CW35" t="s">
+        <v>244</v>
+      </c>
+      <c r="CX35" t="s">
+        <v>244</v>
+      </c>
+      <c r="CY35" t="s">
+        <v>244</v>
+      </c>
+      <c r="CZ35" t="s">
+        <v>244</v>
+      </c>
+      <c r="DA35" t="s">
+        <v>239</v>
+      </c>
+      <c r="DB35" t="s">
+        <v>244</v>
+      </c>
+      <c r="DC35" t="s">
+        <v>651</v>
+      </c>
+      <c r="DD35" t="s">
+        <v>282</v>
+      </c>
+      <c r="DE35" t="s">
+        <v>631</v>
+      </c>
+      <c r="DF35" t="s">
+        <v>632</v>
+      </c>
+      <c r="DG35" t="s">
+        <v>282</v>
+      </c>
+      <c r="DH35" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="36" spans="1:112" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>643</v>
+      </c>
+      <c r="B36" t="s">
+        <v>379</v>
+      </c>
+      <c r="C36" t="s">
+        <v>644</v>
+      </c>
+      <c r="D36" s="1">
+        <v>45839.332997685196</v>
+      </c>
+      <c r="E36" t="s">
+        <v>261</v>
+      </c>
+      <c r="F36" s="1">
+        <v>45842.161956018499</v>
+      </c>
+      <c r="G36" s="1">
+        <v>45856.286967592598</v>
+      </c>
+      <c r="H36" t="s">
+        <v>235</v>
+      </c>
+      <c r="I36" s="1">
+        <v>45839.332664907401</v>
+      </c>
+      <c r="J36" t="s">
+        <v>620</v>
+      </c>
+      <c r="K36" t="s">
+        <v>237</v>
+      </c>
+      <c r="L36" t="s">
+        <v>238</v>
+      </c>
+      <c r="M36" s="2">
+        <v>45832</v>
+      </c>
+      <c r="N36" t="s">
+        <v>239</v>
+      </c>
+      <c r="O36" t="s">
+        <v>240</v>
+      </c>
+      <c r="P36" t="s">
+        <v>400</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>645</v>
+      </c>
+      <c r="R36" t="s">
+        <v>339</v>
+      </c>
+      <c r="S36" t="s">
+        <v>239</v>
+      </c>
+      <c r="T36" t="s">
+        <v>244</v>
+      </c>
+      <c r="U36">
+        <v>314</v>
+      </c>
+      <c r="V36" t="s">
+        <v>245</v>
+      </c>
+      <c r="W36" t="s">
+        <v>304</v>
+      </c>
+      <c r="X36" t="s">
+        <v>247</v>
+      </c>
+      <c r="Y36" t="s">
+        <v>248</v>
+      </c>
+      <c r="Z36" t="s">
+        <v>240</v>
+      </c>
+      <c r="AA36" t="s">
+        <v>249</v>
+      </c>
+      <c r="AB36" t="s">
+        <v>646</v>
+      </c>
+      <c r="AC36" t="s">
+        <v>261</v>
+      </c>
+      <c r="AD36" t="s">
+        <v>546</v>
+      </c>
+      <c r="AE36" t="s">
+        <v>647</v>
+      </c>
+      <c r="AF36" t="s">
+        <v>247</v>
+      </c>
+      <c r="AG36" t="s">
+        <v>248</v>
+      </c>
+      <c r="AH36" t="s">
+        <v>247</v>
+      </c>
+      <c r="AI36" t="s">
+        <v>253</v>
+      </c>
+      <c r="AJ36" t="s">
+        <v>247</v>
+      </c>
+      <c r="AK36" t="s">
+        <v>244</v>
+      </c>
+      <c r="AL36" t="s">
+        <v>449</v>
+      </c>
+      <c r="AM36">
+        <v>15</v>
+      </c>
+      <c r="AN36" t="s">
+        <v>639</v>
+      </c>
+      <c r="AO36" t="s">
+        <v>240</v>
+      </c>
+      <c r="AP36" t="s">
+        <v>244</v>
+      </c>
+      <c r="AQ36">
+        <v>45</v>
+      </c>
+      <c r="AR36">
+        <v>9</v>
+      </c>
+      <c r="AS36" t="s">
+        <v>239</v>
+      </c>
+      <c r="AT36" t="s">
+        <v>257</v>
+      </c>
+      <c r="AU36" t="s">
+        <v>247</v>
+      </c>
+      <c r="AV36" t="s">
+        <v>247</v>
+      </c>
+      <c r="AW36" t="s">
+        <v>247</v>
+      </c>
+      <c r="AX36" t="s">
+        <v>244</v>
+      </c>
+      <c r="AY36" t="s">
+        <v>258</v>
+      </c>
+      <c r="AZ36" t="s">
+        <v>648</v>
+      </c>
+      <c r="BA36" t="s">
+        <v>629</v>
+      </c>
+      <c r="BB36" t="s">
+        <v>261</v>
+      </c>
+      <c r="BC36" t="s">
+        <v>261</v>
+      </c>
+      <c r="BD36" t="s">
+        <v>261</v>
+      </c>
+      <c r="BE36" t="s">
+        <v>261</v>
+      </c>
+      <c r="BF36" t="s">
+        <v>261</v>
+      </c>
+      <c r="BG36" t="s">
+        <v>261</v>
+      </c>
+      <c r="BH36" t="s">
+        <v>261</v>
+      </c>
+      <c r="BI36" t="s">
+        <v>261</v>
+      </c>
+      <c r="BJ36" t="s">
+        <v>261</v>
+      </c>
+      <c r="BK36" t="s">
+        <v>261</v>
+      </c>
+      <c r="BL36" t="s">
+        <v>261</v>
+      </c>
+      <c r="BM36" t="s">
+        <v>261</v>
+      </c>
+      <c r="BN36" t="s">
+        <v>261</v>
+      </c>
+      <c r="BO36" t="s">
+        <v>261</v>
+      </c>
+      <c r="BP36" t="s">
+        <v>261</v>
+      </c>
+      <c r="BQ36" t="s">
+        <v>261</v>
+      </c>
+      <c r="BR36" t="s">
+        <v>261</v>
+      </c>
+      <c r="BS36" t="s">
+        <v>261</v>
+      </c>
+      <c r="BT36" t="s">
+        <v>261</v>
+      </c>
+      <c r="BU36" t="s">
+        <v>261</v>
+      </c>
+      <c r="BV36" t="s">
+        <v>261</v>
+      </c>
+      <c r="BW36" t="s">
+        <v>261</v>
+      </c>
+      <c r="BX36" t="s">
+        <v>261</v>
+      </c>
+      <c r="BY36" t="s">
+        <v>261</v>
+      </c>
+      <c r="BZ36" t="s">
+        <v>261</v>
+      </c>
+      <c r="CA36" t="s">
+        <v>261</v>
+      </c>
+      <c r="CB36" t="s">
+        <v>261</v>
+      </c>
+      <c r="CC36" t="s">
+        <v>261</v>
+      </c>
+      <c r="CD36" t="s">
+        <v>261</v>
+      </c>
+      <c r="CE36" t="s">
+        <v>261</v>
+      </c>
+      <c r="CF36" t="s">
+        <v>261</v>
+      </c>
+      <c r="CG36" t="s">
+        <v>261</v>
+      </c>
+      <c r="CH36" t="s">
+        <v>261</v>
+      </c>
+      <c r="CI36" t="s">
+        <v>261</v>
+      </c>
+      <c r="CJ36" t="s">
+        <v>261</v>
+      </c>
+      <c r="CK36" t="s">
+        <v>261</v>
+      </c>
+      <c r="CL36" t="s">
+        <v>261</v>
+      </c>
+      <c r="CM36" t="s">
+        <v>261</v>
+      </c>
+      <c r="CN36" t="s">
+        <v>261</v>
+      </c>
+      <c r="CO36" t="s">
+        <v>261</v>
+      </c>
+      <c r="CP36" t="s">
+        <v>261</v>
+      </c>
+      <c r="CQ36" t="s">
+        <v>261</v>
+      </c>
+      <c r="CR36">
+        <v>3.1</v>
+      </c>
+      <c r="CS36" t="s">
+        <v>649</v>
+      </c>
+      <c r="CT36">
+        <v>0.78</v>
+      </c>
+      <c r="CU36" t="s">
+        <v>280</v>
+      </c>
+      <c r="CV36" t="s">
+        <v>239</v>
+      </c>
+      <c r="CW36" t="s">
+        <v>244</v>
+      </c>
+      <c r="CX36" t="s">
+        <v>244</v>
+      </c>
+      <c r="CY36" t="s">
+        <v>244</v>
+      </c>
+      <c r="CZ36" t="s">
+        <v>244</v>
+      </c>
+      <c r="DA36" t="s">
+        <v>239</v>
+      </c>
+      <c r="DB36" t="s">
+        <v>244</v>
+      </c>
+      <c r="DC36" t="s">
+        <v>652</v>
+      </c>
+      <c r="DD36" t="s">
+        <v>282</v>
+      </c>
+      <c r="DE36" t="s">
+        <v>453</v>
+      </c>
+      <c r="DF36" t="s">
+        <v>632</v>
+      </c>
+      <c r="DG36" t="s">
+        <v>282</v>
+      </c>
+      <c r="DH36" t="s">
         <v>282</v>
       </c>
     </row>

</xml_diff>